<commit_message>
added second auxiliary file to convert 24-h series by month (e.g. for downstream irrigation needs) to full hourly timeseries
</commit_message>
<xml_diff>
--- a/data/auxiliary scripts/rearrange_data_template.xlsx
+++ b/data/auxiliary scripts/rearrange_data_template.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/auxiliary scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C831CF-FC61-4E26-9E39-5C9BFFF5D697}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20F54EE2-82EC-4F9E-A3AA-03552BE4A699}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F0237BE4-5998-4954-96A9-CCA6E6B1B117}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F0237BE4-5998-4954-96A9-CCA6E6B1B117}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly_series" sheetId="3" r:id="rId1"/>
+    <sheet name="daily_bymonth_series" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="505">
   <si>
     <t>first_year</t>
   </si>
@@ -668,17 +669,896 @@
     <t>series 3 (e.g. precipitation)</t>
   </si>
   <si>
-    <t>(enter monthly data here, then run script rearrange_data_monthly_to_hourly.py to convert to hourly matrices "output_hourly_byyear" for REVUB input)</t>
-  </si>
-  <si>
     <t>activate for conversion (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>activate for conversion</t>
+  </si>
+  <si>
+    <t>Jan 0h</t>
+  </si>
+  <si>
+    <t>Jan 1h</t>
+  </si>
+  <si>
+    <t>Jan 2h</t>
+  </si>
+  <si>
+    <t>Jan 3h</t>
+  </si>
+  <si>
+    <t>Jan 4h</t>
+  </si>
+  <si>
+    <t>Jan 5h</t>
+  </si>
+  <si>
+    <t>Jan 6h</t>
+  </si>
+  <si>
+    <t>Jan 7h</t>
+  </si>
+  <si>
+    <t>Jan 8h</t>
+  </si>
+  <si>
+    <t>Jan 9h</t>
+  </si>
+  <si>
+    <t>Jan 10h</t>
+  </si>
+  <si>
+    <t>Jan 11h</t>
+  </si>
+  <si>
+    <t>Jan 12h</t>
+  </si>
+  <si>
+    <t>Jan 13h</t>
+  </si>
+  <si>
+    <t>Jan 14h</t>
+  </si>
+  <si>
+    <t>Jan 15h</t>
+  </si>
+  <si>
+    <t>Jan 16h</t>
+  </si>
+  <si>
+    <t>Jan 17h</t>
+  </si>
+  <si>
+    <t>Jan 18h</t>
+  </si>
+  <si>
+    <t>Jan 19h</t>
+  </si>
+  <si>
+    <t>Jan 20h</t>
+  </si>
+  <si>
+    <t>Jan 21h</t>
+  </si>
+  <si>
+    <t>Jan 22h</t>
+  </si>
+  <si>
+    <t>Jan 23h</t>
+  </si>
+  <si>
+    <t>Feb 0h</t>
+  </si>
+  <si>
+    <t>Feb 1h</t>
+  </si>
+  <si>
+    <t>Feb 2h</t>
+  </si>
+  <si>
+    <t>Feb 3h</t>
+  </si>
+  <si>
+    <t>Feb 4h</t>
+  </si>
+  <si>
+    <t>Feb 5h</t>
+  </si>
+  <si>
+    <t>Feb 6h</t>
+  </si>
+  <si>
+    <t>Feb 7h</t>
+  </si>
+  <si>
+    <t>Feb 8h</t>
+  </si>
+  <si>
+    <t>Feb 9h</t>
+  </si>
+  <si>
+    <t>Feb 10h</t>
+  </si>
+  <si>
+    <t>Feb 11h</t>
+  </si>
+  <si>
+    <t>Feb 12h</t>
+  </si>
+  <si>
+    <t>Feb 13h</t>
+  </si>
+  <si>
+    <t>Feb 14h</t>
+  </si>
+  <si>
+    <t>Feb 15h</t>
+  </si>
+  <si>
+    <t>Feb 16h</t>
+  </si>
+  <si>
+    <t>Feb 17h</t>
+  </si>
+  <si>
+    <t>Feb 18h</t>
+  </si>
+  <si>
+    <t>Feb 19h</t>
+  </si>
+  <si>
+    <t>Feb 20h</t>
+  </si>
+  <si>
+    <t>Feb 21h</t>
+  </si>
+  <si>
+    <t>Feb 22h</t>
+  </si>
+  <si>
+    <t>Feb 23h</t>
+  </si>
+  <si>
+    <t>Mar 0h</t>
+  </si>
+  <si>
+    <t>Mar 1h</t>
+  </si>
+  <si>
+    <t>Mar 2h</t>
+  </si>
+  <si>
+    <t>Mar 3h</t>
+  </si>
+  <si>
+    <t>Mar 4h</t>
+  </si>
+  <si>
+    <t>Mar 5h</t>
+  </si>
+  <si>
+    <t>Mar 6h</t>
+  </si>
+  <si>
+    <t>Mar 7h</t>
+  </si>
+  <si>
+    <t>Mar 8h</t>
+  </si>
+  <si>
+    <t>Mar 9h</t>
+  </si>
+  <si>
+    <t>Mar 10h</t>
+  </si>
+  <si>
+    <t>Mar 11h</t>
+  </si>
+  <si>
+    <t>Mar 12h</t>
+  </si>
+  <si>
+    <t>Mar 13h</t>
+  </si>
+  <si>
+    <t>Mar 14h</t>
+  </si>
+  <si>
+    <t>Mar 15h</t>
+  </si>
+  <si>
+    <t>Mar 16h</t>
+  </si>
+  <si>
+    <t>Mar 17h</t>
+  </si>
+  <si>
+    <t>Mar 18h</t>
+  </si>
+  <si>
+    <t>Mar 19h</t>
+  </si>
+  <si>
+    <t>Mar 20h</t>
+  </si>
+  <si>
+    <t>Mar 21h</t>
+  </si>
+  <si>
+    <t>Mar 22h</t>
+  </si>
+  <si>
+    <t>Mar 23h</t>
+  </si>
+  <si>
+    <t>Apr 0h</t>
+  </si>
+  <si>
+    <t>Apr 1h</t>
+  </si>
+  <si>
+    <t>Apr 2h</t>
+  </si>
+  <si>
+    <t>Apr 3h</t>
+  </si>
+  <si>
+    <t>Apr 4h</t>
+  </si>
+  <si>
+    <t>Apr 5h</t>
+  </si>
+  <si>
+    <t>Apr 6h</t>
+  </si>
+  <si>
+    <t>Apr 7h</t>
+  </si>
+  <si>
+    <t>Apr 8h</t>
+  </si>
+  <si>
+    <t>Apr 9h</t>
+  </si>
+  <si>
+    <t>Apr 10h</t>
+  </si>
+  <si>
+    <t>Apr 11h</t>
+  </si>
+  <si>
+    <t>Apr 12h</t>
+  </si>
+  <si>
+    <t>Apr 13h</t>
+  </si>
+  <si>
+    <t>Apr 14h</t>
+  </si>
+  <si>
+    <t>Apr 15h</t>
+  </si>
+  <si>
+    <t>Apr 16h</t>
+  </si>
+  <si>
+    <t>Apr 17h</t>
+  </si>
+  <si>
+    <t>Apr 18h</t>
+  </si>
+  <si>
+    <t>Apr 19h</t>
+  </si>
+  <si>
+    <t>Apr 20h</t>
+  </si>
+  <si>
+    <t>Apr 21h</t>
+  </si>
+  <si>
+    <t>Apr 22h</t>
+  </si>
+  <si>
+    <t>Apr 23h</t>
+  </si>
+  <si>
+    <t>May 0h</t>
+  </si>
+  <si>
+    <t>May 1h</t>
+  </si>
+  <si>
+    <t>May 2h</t>
+  </si>
+  <si>
+    <t>May 3h</t>
+  </si>
+  <si>
+    <t>May 4h</t>
+  </si>
+  <si>
+    <t>May 5h</t>
+  </si>
+  <si>
+    <t>May 6h</t>
+  </si>
+  <si>
+    <t>May 7h</t>
+  </si>
+  <si>
+    <t>May 8h</t>
+  </si>
+  <si>
+    <t>May 9h</t>
+  </si>
+  <si>
+    <t>May 10h</t>
+  </si>
+  <si>
+    <t>May 11h</t>
+  </si>
+  <si>
+    <t>May 12h</t>
+  </si>
+  <si>
+    <t>May 13h</t>
+  </si>
+  <si>
+    <t>May 14h</t>
+  </si>
+  <si>
+    <t>May 15h</t>
+  </si>
+  <si>
+    <t>May 16h</t>
+  </si>
+  <si>
+    <t>May 17h</t>
+  </si>
+  <si>
+    <t>May 18h</t>
+  </si>
+  <si>
+    <t>May 19h</t>
+  </si>
+  <si>
+    <t>May 20h</t>
+  </si>
+  <si>
+    <t>May 21h</t>
+  </si>
+  <si>
+    <t>May 22h</t>
+  </si>
+  <si>
+    <t>May 23h</t>
+  </si>
+  <si>
+    <t>Jun 0h</t>
+  </si>
+  <si>
+    <t>Jun 1h</t>
+  </si>
+  <si>
+    <t>Jun 2h</t>
+  </si>
+  <si>
+    <t>Jun 3h</t>
+  </si>
+  <si>
+    <t>Jun 4h</t>
+  </si>
+  <si>
+    <t>Jun 5h</t>
+  </si>
+  <si>
+    <t>Jun 6h</t>
+  </si>
+  <si>
+    <t>Jun 7h</t>
+  </si>
+  <si>
+    <t>Jun 8h</t>
+  </si>
+  <si>
+    <t>Jun 9h</t>
+  </si>
+  <si>
+    <t>Jun 10h</t>
+  </si>
+  <si>
+    <t>Jun 11h</t>
+  </si>
+  <si>
+    <t>Jun 12h</t>
+  </si>
+  <si>
+    <t>Jun 13h</t>
+  </si>
+  <si>
+    <t>Jun 14h</t>
+  </si>
+  <si>
+    <t>Jun 15h</t>
+  </si>
+  <si>
+    <t>Jun 16h</t>
+  </si>
+  <si>
+    <t>Jun 17h</t>
+  </si>
+  <si>
+    <t>Jun 18h</t>
+  </si>
+  <si>
+    <t>Jun 19h</t>
+  </si>
+  <si>
+    <t>Jun 20h</t>
+  </si>
+  <si>
+    <t>Jun 21h</t>
+  </si>
+  <si>
+    <t>Jun 22h</t>
+  </si>
+  <si>
+    <t>Jun 23h</t>
+  </si>
+  <si>
+    <t>Jul 0h</t>
+  </si>
+  <si>
+    <t>Jul 1h</t>
+  </si>
+  <si>
+    <t>Jul 2h</t>
+  </si>
+  <si>
+    <t>Jul 3h</t>
+  </si>
+  <si>
+    <t>Jul 4h</t>
+  </si>
+  <si>
+    <t>Jul 5h</t>
+  </si>
+  <si>
+    <t>Jul 6h</t>
+  </si>
+  <si>
+    <t>Jul 7h</t>
+  </si>
+  <si>
+    <t>Jul 8h</t>
+  </si>
+  <si>
+    <t>Jul 9h</t>
+  </si>
+  <si>
+    <t>Jul 10h</t>
+  </si>
+  <si>
+    <t>Jul 11h</t>
+  </si>
+  <si>
+    <t>Jul 12h</t>
+  </si>
+  <si>
+    <t>Jul 13h</t>
+  </si>
+  <si>
+    <t>Jul 14h</t>
+  </si>
+  <si>
+    <t>Jul 15h</t>
+  </si>
+  <si>
+    <t>Jul 16h</t>
+  </si>
+  <si>
+    <t>Jul 17h</t>
+  </si>
+  <si>
+    <t>Jul 18h</t>
+  </si>
+  <si>
+    <t>Jul 19h</t>
+  </si>
+  <si>
+    <t>Jul 20h</t>
+  </si>
+  <si>
+    <t>Jul 21h</t>
+  </si>
+  <si>
+    <t>Jul 22h</t>
+  </si>
+  <si>
+    <t>Jul 23h</t>
+  </si>
+  <si>
+    <t>Aug 0h</t>
+  </si>
+  <si>
+    <t>Aug 1h</t>
+  </si>
+  <si>
+    <t>Aug 2h</t>
+  </si>
+  <si>
+    <t>Aug 3h</t>
+  </si>
+  <si>
+    <t>Aug 4h</t>
+  </si>
+  <si>
+    <t>Aug 5h</t>
+  </si>
+  <si>
+    <t>Aug 6h</t>
+  </si>
+  <si>
+    <t>Aug 7h</t>
+  </si>
+  <si>
+    <t>Aug 8h</t>
+  </si>
+  <si>
+    <t>Aug 9h</t>
+  </si>
+  <si>
+    <t>Aug 10h</t>
+  </si>
+  <si>
+    <t>Aug 11h</t>
+  </si>
+  <si>
+    <t>Aug 12h</t>
+  </si>
+  <si>
+    <t>Aug 13h</t>
+  </si>
+  <si>
+    <t>Aug 14h</t>
+  </si>
+  <si>
+    <t>Aug 15h</t>
+  </si>
+  <si>
+    <t>Aug 16h</t>
+  </si>
+  <si>
+    <t>Aug 17h</t>
+  </si>
+  <si>
+    <t>Aug 18h</t>
+  </si>
+  <si>
+    <t>Aug 19h</t>
+  </si>
+  <si>
+    <t>Aug 20h</t>
+  </si>
+  <si>
+    <t>Aug 21h</t>
+  </si>
+  <si>
+    <t>Aug 22h</t>
+  </si>
+  <si>
+    <t>Aug 23h</t>
+  </si>
+  <si>
+    <t>Sep 0h</t>
+  </si>
+  <si>
+    <t>Sep 1h</t>
+  </si>
+  <si>
+    <t>Sep 2h</t>
+  </si>
+  <si>
+    <t>Sep 3h</t>
+  </si>
+  <si>
+    <t>Sep 4h</t>
+  </si>
+  <si>
+    <t>Sep 5h</t>
+  </si>
+  <si>
+    <t>Sep 6h</t>
+  </si>
+  <si>
+    <t>Sep 7h</t>
+  </si>
+  <si>
+    <t>Sep 8h</t>
+  </si>
+  <si>
+    <t>Sep 9h</t>
+  </si>
+  <si>
+    <t>Sep 10h</t>
+  </si>
+  <si>
+    <t>Sep 11h</t>
+  </si>
+  <si>
+    <t>Sep 12h</t>
+  </si>
+  <si>
+    <t>Sep 13h</t>
+  </si>
+  <si>
+    <t>Sep 14h</t>
+  </si>
+  <si>
+    <t>Sep 15h</t>
+  </si>
+  <si>
+    <t>Sep 16h</t>
+  </si>
+  <si>
+    <t>Sep 17h</t>
+  </si>
+  <si>
+    <t>Sep 18h</t>
+  </si>
+  <si>
+    <t>Sep 19h</t>
+  </si>
+  <si>
+    <t>Sep 20h</t>
+  </si>
+  <si>
+    <t>Sep 21h</t>
+  </si>
+  <si>
+    <t>Sep 22h</t>
+  </si>
+  <si>
+    <t>Sep 23h</t>
+  </si>
+  <si>
+    <t>Oct 0h</t>
+  </si>
+  <si>
+    <t>Oct 1h</t>
+  </si>
+  <si>
+    <t>Oct 2h</t>
+  </si>
+  <si>
+    <t>Oct 3h</t>
+  </si>
+  <si>
+    <t>Oct 4h</t>
+  </si>
+  <si>
+    <t>Oct 5h</t>
+  </si>
+  <si>
+    <t>Oct 6h</t>
+  </si>
+  <si>
+    <t>Oct 7h</t>
+  </si>
+  <si>
+    <t>Oct 8h</t>
+  </si>
+  <si>
+    <t>Oct 9h</t>
+  </si>
+  <si>
+    <t>Oct 10h</t>
+  </si>
+  <si>
+    <t>Oct 11h</t>
+  </si>
+  <si>
+    <t>Oct 12h</t>
+  </si>
+  <si>
+    <t>Oct 13h</t>
+  </si>
+  <si>
+    <t>Oct 14h</t>
+  </si>
+  <si>
+    <t>Oct 15h</t>
+  </si>
+  <si>
+    <t>Oct 16h</t>
+  </si>
+  <si>
+    <t>Oct 17h</t>
+  </si>
+  <si>
+    <t>Oct 18h</t>
+  </si>
+  <si>
+    <t>Oct 19h</t>
+  </si>
+  <si>
+    <t>Oct 20h</t>
+  </si>
+  <si>
+    <t>Oct 21h</t>
+  </si>
+  <si>
+    <t>Oct 22h</t>
+  </si>
+  <si>
+    <t>Oct 23h</t>
+  </si>
+  <si>
+    <t>Nov 0h</t>
+  </si>
+  <si>
+    <t>Nov 1h</t>
+  </si>
+  <si>
+    <t>Nov 2h</t>
+  </si>
+  <si>
+    <t>Nov 3h</t>
+  </si>
+  <si>
+    <t>Nov 4h</t>
+  </si>
+  <si>
+    <t>Nov 5h</t>
+  </si>
+  <si>
+    <t>Nov 6h</t>
+  </si>
+  <si>
+    <t>Nov 7h</t>
+  </si>
+  <si>
+    <t>Nov 8h</t>
+  </si>
+  <si>
+    <t>Nov 9h</t>
+  </si>
+  <si>
+    <t>Nov 10h</t>
+  </si>
+  <si>
+    <t>Nov 11h</t>
+  </si>
+  <si>
+    <t>Nov 12h</t>
+  </si>
+  <si>
+    <t>Nov 13h</t>
+  </si>
+  <si>
+    <t>Nov 14h</t>
+  </si>
+  <si>
+    <t>Nov 15h</t>
+  </si>
+  <si>
+    <t>Nov 16h</t>
+  </si>
+  <si>
+    <t>Nov 17h</t>
+  </si>
+  <si>
+    <t>Nov 18h</t>
+  </si>
+  <si>
+    <t>Nov 19h</t>
+  </si>
+  <si>
+    <t>Nov 20h</t>
+  </si>
+  <si>
+    <t>Nov 21h</t>
+  </si>
+  <si>
+    <t>Nov 22h</t>
+  </si>
+  <si>
+    <t>Nov 23h</t>
+  </si>
+  <si>
+    <t>Dec 0h</t>
+  </si>
+  <si>
+    <t>Dec 1h</t>
+  </si>
+  <si>
+    <t>Dec 2h</t>
+  </si>
+  <si>
+    <t>Dec 3h</t>
+  </si>
+  <si>
+    <t>Dec 4h</t>
+  </si>
+  <si>
+    <t>Dec 5h</t>
+  </si>
+  <si>
+    <t>Dec 6h</t>
+  </si>
+  <si>
+    <t>Dec 7h</t>
+  </si>
+  <si>
+    <t>Dec 8h</t>
+  </si>
+  <si>
+    <t>Dec 9h</t>
+  </si>
+  <si>
+    <t>Dec 10h</t>
+  </si>
+  <si>
+    <t>Dec 11h</t>
+  </si>
+  <si>
+    <t>Dec 12h</t>
+  </si>
+  <si>
+    <t>Dec 13h</t>
+  </si>
+  <si>
+    <t>Dec 14h</t>
+  </si>
+  <si>
+    <t>Dec 15h</t>
+  </si>
+  <si>
+    <t>Dec 16h</t>
+  </si>
+  <si>
+    <t>Dec 17h</t>
+  </si>
+  <si>
+    <t>Dec 18h</t>
+  </si>
+  <si>
+    <t>Dec 19h</t>
+  </si>
+  <si>
+    <t>Dec 20h</t>
+  </si>
+  <si>
+    <t>Dec 21h</t>
+  </si>
+  <si>
+    <t>Dec 22h</t>
+  </si>
+  <si>
+    <t>Dec 23h</t>
+  </si>
+  <si>
+    <t>series A (e.g. irrigation needs downstream of plant A)</t>
+  </si>
+  <si>
+    <t>series B (e.g. irrigation needs downstream of plant B)</t>
+  </si>
+  <si>
+    <t>(enter monthly data here [starting in January], then run script rearrange_data_monthly_to_hourly.py to convert to hourly matrices "output_hourly_byyear" for REVUB input)</t>
+  </si>
+  <si>
+    <t>(note: the data in column A may have to be manually extended/shortened depending on the first_year and last_year parameters)</t>
+  </si>
+  <si>
+    <t>(enter hourly data here for each month, then run script rearrange_data_daily_bymonth_to_hourly.py to convert to hourly matrices "output_hourly_byyear" for REVUB input)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,6 +1576,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -721,11 +1609,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1042,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C021A5-F7BC-4443-80E5-F6F0685F792B}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,7 +1963,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1115,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>210</v>
+        <v>502</v>
       </c>
       <c r="D5" s="1"/>
       <c r="H5" s="1"/>
@@ -1124,6 +2017,9 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2141,4 +3037,1511 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF5CBF9-CA84-41E1-BA39-076243C43A9E}">
+  <dimension ref="A1:C292"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1998</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" s="5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" s="5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A206" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A226" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A238" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A239" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A240" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A241" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A242" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A243" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A244" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A245" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A246" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A247" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A248" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A249" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A250" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A251" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A252" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A253" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A254" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A255" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A256" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A257" s="5" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A258" s="5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A259" s="5" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" s="5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A261" s="5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A262" s="5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A263" s="5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A264" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A265" s="5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A266" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A267" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A268" s="5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A269" s="5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A270" s="5" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A272" s="5" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A273" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A274" s="5" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A275" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A276" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A277" s="5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A278" s="5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A279" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A280" s="5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A282" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A283" s="5" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A284" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A285" s="5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A286" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A287" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A288" s="5" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A289" s="5" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A290" s="5" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A291" s="5" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A292" s="5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
small cosmetic corrections to code and input sheets
</commit_message>
<xml_diff>
--- a/data/auxiliary scripts/rearrange_data_template.xlsx
+++ b/data/auxiliary scripts/rearrange_data_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/auxiliary scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20F54EE2-82EC-4F9E-A3AA-03552BE4A699}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A05E94F-8572-4DA4-9BAD-27F0FA8DA1BC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F0237BE4-5998-4954-96A9-CCA6E6B1B117}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="504">
   <si>
     <t>first_year</t>
   </si>
@@ -670,9 +670,6 @@
   </si>
   <si>
     <t>activate for conversion (1 = yes, 0 = no)</t>
-  </si>
-  <si>
-    <t>activate for conversion</t>
   </si>
   <si>
     <t>Jan 0h</t>
@@ -1637,9 +1634,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1677,7 +1674,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1783,7 +1780,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1925,7 +1922,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1936,7 +1933,7 @@
   <dimension ref="A1:I208"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,7 +2005,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D5" s="1"/>
       <c r="H5" s="1"/>
@@ -2019,7 +2016,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3044,7 +3041,7 @@
   <dimension ref="A1:C292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3059,15 +3056,15 @@
         <v>206</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3100,1445 +3097,1445 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A265" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A267" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A281" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A288" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A289" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A290" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A291" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A292" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colour coding introduction in Excel control files
</commit_message>
<xml_diff>
--- a/data/auxiliary scripts/rearrange_data_template.xlsx
+++ b/data/auxiliary scripts/rearrange_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/auxiliary scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A05E94F-8572-4DA4-9BAD-27F0FA8DA1BC}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{1FE34037-6CD7-4854-90B7-96CD817059A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A14019-4BE3-4647-B860-CD01E332C662}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F0237BE4-5998-4954-96A9-CCA6E6B1B117}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F0237BE4-5998-4954-96A9-CCA6E6B1B117}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly_series" sheetId="3" r:id="rId1"/>
@@ -1555,7 +1555,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1578,23 +1578,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1602,23 +1618,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1631,6 +1682,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1932,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C021A5-F7BC-4443-80E5-F6F0685F792B}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1944,59 +1999,59 @@
     <col min="4" max="4" width="23.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>206</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>210</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7">
         <v>1998</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>1998</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>1998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>2014</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>2014</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>2014</v>
       </c>
     </row>
@@ -3040,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF5CBF9-CA84-41E1-BA39-076243C43A9E}">
   <dimension ref="A1:C292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3051,52 +3106,52 @@
     <col min="3" max="3" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>210</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="7">
         <v>1998</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>1998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="7">
         <v>2014</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="7">
         <v>2014</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>211</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -3104,1437 +3159,1437 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="4" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="4" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="4" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="4" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="4" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="4" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="4" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="4" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="4" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="4" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="4" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="4" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="4" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="4" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="4" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="4" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="4" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="4" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="4" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="4" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="4" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="4" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="4" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="4" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="4" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="4" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="4" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="4" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="4" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="4" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="4" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="4" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="4" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="4" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="4" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="4" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="4" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="4" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="4" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="4" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="4" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="4" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="4" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="4" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="4" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="4" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="4" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="4" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="4" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A136" s="5" t="s">
+      <c r="A136" s="4" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="4" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A138" s="5" t="s">
+      <c r="A138" s="4" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A139" s="5" t="s">
+      <c r="A139" s="4" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="4" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A141" s="5" t="s">
+      <c r="A141" s="4" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="4" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A143" s="5" t="s">
+      <c r="A143" s="4" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A144" s="5" t="s">
+      <c r="A144" s="4" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="5" t="s">
+      <c r="A145" s="4" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A146" s="5" t="s">
+      <c r="A146" s="4" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A147" s="5" t="s">
+      <c r="A147" s="4" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A148" s="5" t="s">
+      <c r="A148" s="4" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A149" s="5" t="s">
+      <c r="A149" s="4" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A150" s="5" t="s">
+      <c r="A150" s="4" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A151" s="5" t="s">
+      <c r="A151" s="4" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A152" s="5" t="s">
+      <c r="A152" s="4" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A153" s="5" t="s">
+      <c r="A153" s="4" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A154" s="5" t="s">
+      <c r="A154" s="4" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A155" s="5" t="s">
+      <c r="A155" s="4" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A156" s="5" t="s">
+      <c r="A156" s="4" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A157" s="5" t="s">
+      <c r="A157" s="4" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A158" s="5" t="s">
+      <c r="A158" s="4" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A159" s="5" t="s">
+      <c r="A159" s="4" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A160" s="5" t="s">
+      <c r="A160" s="4" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A161" s="5" t="s">
+      <c r="A161" s="4" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A162" s="5" t="s">
+      <c r="A162" s="4" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A163" s="5" t="s">
+      <c r="A163" s="4" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A164" s="5" t="s">
+      <c r="A164" s="4" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A165" s="5" t="s">
+      <c r="A165" s="4" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A166" s="5" t="s">
+      <c r="A166" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A167" s="5" t="s">
+      <c r="A167" s="4" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A168" s="5" t="s">
+      <c r="A168" s="4" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A169" s="5" t="s">
+      <c r="A169" s="4" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A170" s="5" t="s">
+      <c r="A170" s="4" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A171" s="5" t="s">
+      <c r="A171" s="4" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A172" s="5" t="s">
+      <c r="A172" s="4" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A173" s="5" t="s">
+      <c r="A173" s="4" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A174" s="5" t="s">
+      <c r="A174" s="4" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A175" s="5" t="s">
+      <c r="A175" s="4" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A176" s="5" t="s">
+      <c r="A176" s="4" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A177" s="5" t="s">
+      <c r="A177" s="4" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A178" s="5" t="s">
+      <c r="A178" s="4" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A179" s="5" t="s">
+      <c r="A179" s="4" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A180" s="5" t="s">
+      <c r="A180" s="4" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A181" s="5" t="s">
+      <c r="A181" s="4" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A182" s="5" t="s">
+      <c r="A182" s="4" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A183" s="5" t="s">
+      <c r="A183" s="4" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A184" s="5" t="s">
+      <c r="A184" s="4" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A185" s="5" t="s">
+      <c r="A185" s="4" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A186" s="5" t="s">
+      <c r="A186" s="4" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A187" s="5" t="s">
+      <c r="A187" s="4" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A188" s="5" t="s">
+      <c r="A188" s="4" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A189" s="5" t="s">
+      <c r="A189" s="4" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A190" s="5" t="s">
+      <c r="A190" s="4" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A191" s="5" t="s">
+      <c r="A191" s="4" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A192" s="5" t="s">
+      <c r="A192" s="4" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A193" s="5" t="s">
+      <c r="A193" s="4" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A194" s="5" t="s">
+      <c r="A194" s="4" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A195" s="5" t="s">
+      <c r="A195" s="4" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A196" s="5" t="s">
+      <c r="A196" s="4" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A197" s="5" t="s">
+      <c r="A197" s="4" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A198" s="5" t="s">
+      <c r="A198" s="4" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A199" s="5" t="s">
+      <c r="A199" s="4" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A200" s="5" t="s">
+      <c r="A200" s="4" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A201" s="5" t="s">
+      <c r="A201" s="4" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A202" s="5" t="s">
+      <c r="A202" s="4" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A203" s="5" t="s">
+      <c r="A203" s="4" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A204" s="5" t="s">
+      <c r="A204" s="4" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A205" s="5" t="s">
+      <c r="A205" s="4" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A206" s="5" t="s">
+      <c r="A206" s="4" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A207" s="5" t="s">
+      <c r="A207" s="4" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A208" s="5" t="s">
+      <c r="A208" s="4" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A209" s="5" t="s">
+      <c r="A209" s="4" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A210" s="5" t="s">
+      <c r="A210" s="4" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A211" s="5" t="s">
+      <c r="A211" s="4" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A212" s="5" t="s">
+      <c r="A212" s="4" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A213" s="5" t="s">
+      <c r="A213" s="4" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A214" s="5" t="s">
+      <c r="A214" s="4" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A215" s="5" t="s">
+      <c r="A215" s="4" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A216" s="5" t="s">
+      <c r="A216" s="4" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A217" s="5" t="s">
+      <c r="A217" s="4" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A218" s="5" t="s">
+      <c r="A218" s="4" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A219" s="5" t="s">
+      <c r="A219" s="4" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A220" s="5" t="s">
+      <c r="A220" s="4" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A221" s="5" t="s">
+      <c r="A221" s="4" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A222" s="5" t="s">
+      <c r="A222" s="4" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A223" s="5" t="s">
+      <c r="A223" s="4" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A224" s="5" t="s">
+      <c r="A224" s="4" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A225" s="5" t="s">
+      <c r="A225" s="4" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A226" s="5" t="s">
+      <c r="A226" s="4" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A227" s="5" t="s">
+      <c r="A227" s="4" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A228" s="5" t="s">
+      <c r="A228" s="4" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A229" s="5" t="s">
+      <c r="A229" s="4" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A230" s="5" t="s">
+      <c r="A230" s="4" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A231" s="5" t="s">
+      <c r="A231" s="4" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A232" s="5" t="s">
+      <c r="A232" s="4" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="4" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A234" s="5" t="s">
+      <c r="A234" s="4" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A235" s="5" t="s">
+      <c r="A235" s="4" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A236" s="5" t="s">
+      <c r="A236" s="4" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A237" s="5" t="s">
+      <c r="A237" s="4" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A238" s="5" t="s">
+      <c r="A238" s="4" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A239" s="5" t="s">
+      <c r="A239" s="4" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A240" s="5" t="s">
+      <c r="A240" s="4" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A241" s="5" t="s">
+      <c r="A241" s="4" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A242" s="5" t="s">
+      <c r="A242" s="4" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A243" s="5" t="s">
+      <c r="A243" s="4" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A244" s="5" t="s">
+      <c r="A244" s="4" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A245" s="5" t="s">
+      <c r="A245" s="4" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A246" s="5" t="s">
+      <c r="A246" s="4" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A247" s="5" t="s">
+      <c r="A247" s="4" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A248" s="5" t="s">
+      <c r="A248" s="4" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A249" s="5" t="s">
+      <c r="A249" s="4" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A250" s="5" t="s">
+      <c r="A250" s="4" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A251" s="5" t="s">
+      <c r="A251" s="4" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A252" s="5" t="s">
+      <c r="A252" s="4" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A253" s="5" t="s">
+      <c r="A253" s="4" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A254" s="5" t="s">
+      <c r="A254" s="4" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A255" s="5" t="s">
+      <c r="A255" s="4" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A256" s="5" t="s">
+      <c r="A256" s="4" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A257" s="5" t="s">
+      <c r="A257" s="4" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A258" s="5" t="s">
+      <c r="A258" s="4" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A259" s="5" t="s">
+      <c r="A259" s="4" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A260" s="5" t="s">
+      <c r="A260" s="4" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A261" s="5" t="s">
+      <c r="A261" s="4" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A262" s="5" t="s">
+      <c r="A262" s="4" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A263" s="5" t="s">
+      <c r="A263" s="4" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A264" s="5" t="s">
+      <c r="A264" s="4" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A265" s="5" t="s">
+      <c r="A265" s="4" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A266" s="5" t="s">
+      <c r="A266" s="4" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A267" s="5" t="s">
+      <c r="A267" s="4" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A268" s="5" t="s">
+      <c r="A268" s="4" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A269" s="5" t="s">
+      <c r="A269" s="4" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A270" s="5" t="s">
+      <c r="A270" s="4" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A271" s="5" t="s">
+      <c r="A271" s="4" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A272" s="5" t="s">
+      <c r="A272" s="4" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A273" s="5" t="s">
+      <c r="A273" s="4" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A274" s="5" t="s">
+      <c r="A274" s="4" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A275" s="5" t="s">
+      <c r="A275" s="4" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A276" s="5" t="s">
+      <c r="A276" s="4" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A277" s="5" t="s">
+      <c r="A277" s="4" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A278" s="5" t="s">
+      <c r="A278" s="4" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A279" s="5" t="s">
+      <c r="A279" s="4" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A280" s="5" t="s">
+      <c r="A280" s="4" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A281" s="5" t="s">
+      <c r="A281" s="4" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A282" s="5" t="s">
+      <c r="A282" s="4" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A283" s="5" t="s">
+      <c r="A283" s="4" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A284" s="5" t="s">
+      <c r="A284" s="4" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A285" s="5" t="s">
+      <c r="A285" s="4" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A286" s="5" t="s">
+      <c r="A286" s="4" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A287" s="5" t="s">
+      <c r="A287" s="4" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A288" s="5" t="s">
+      <c r="A288" s="4" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A289" s="5" t="s">
+      <c r="A289" s="4" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A290" s="5" t="s">
+      <c r="A290" s="4" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A291" s="5" t="s">
+      <c r="A291" s="4" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A292" s="5" t="s">
+      <c r="A292" s="4" t="s">
         <v>498</v>
       </c>
     </row>

</xml_diff>